<commit_message>
Update test for UFT One
</commit_message>
<xml_diff>
--- a/tests/UFT One Test/UFT One Test/Default.xlsx
+++ b/tests/UFT One Test/UFT One Test/Default.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Action1" sheetId="2" r:id="rId2"/>
-    <sheet name="Action2" sheetId="3" r:id="rId3"/>
+    <sheet name="Version 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Version 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -471,7 +471,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -479,7 +479,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -517,7 +517,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>